<commit_message>
Literature reviews are added. Differential.m is added, visualizing the surface plot of partial derivatives
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4AA73D-8AD9-424C-AF6D-DECDCDD3EFCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55C6A3-94C6-4A29-B812-668969BD545C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Sensor and measurement, fault detection</t>
   </si>
@@ -61,9 +61,6 @@
     <t>https://findit.dtu.dk/en/catalog/230618367</t>
   </si>
   <si>
-    <t xml:space="preserve">Fault diagnosis with ANN </t>
-  </si>
-  <si>
     <t>https://findit.dtu.dk/en/catalog/273389845</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>https://findit.dtu.dk/en/catalog/2289746875</t>
   </si>
   <si>
-    <t xml:space="preserve">Low charge detection </t>
-  </si>
-  <si>
     <t>https://findit.dtu.dk/en/catalog/2391171426</t>
   </si>
   <si>
@@ -236,6 +230,84 @@
   </si>
   <si>
     <t>TCO minimization</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Steady state thermodynamical and empirical equations are used with linear regression, to find the mass flow rate in a single level HVAC system. 6 sensors are used for heating and 4 for cooling. Wild range of operating conditions.</t>
+  </si>
+  <si>
+    <t>HVAC. Empirical and further ANSI/ARI 540-1999 equations are used to find mass flow rates. Linear regression is used. Different equations were needed for different components, eg for fixed and variable speed compressors. For the TXV valve, analytic equations are used. Bayesian log likelihood estimation was used to find if there is fault. The refrigerant flow faults are correctly decoupled from other faults.</t>
+  </si>
+  <si>
+    <t>Linear analytic equations were used to find the location of sensors in the refrigerant cycle. A test signal at a given frequency was used (active identification, in a range which is not too corrupted by disturbances and noise) to configure. Assuming that the frequency signal acts with different magnitudes on the measurements of different signals, GLRT was used to identify sensors. A weight matrix was used on the residuals to reduce the effect of the residuals at the test frequency.  Lab experiments showed worse results than simulation ones.</t>
+  </si>
+  <si>
+    <t>Fault diagnosis with ANN and fuzzy</t>
+  </si>
+  <si>
+    <t>Linguistic rules determined a rule base, upon which an ANN was built. 7 different faults were detected and isolated. The method gives linguistic decisive functions. Sensor malfunctions were identified as well. False positive rates were not checked.</t>
+  </si>
+  <si>
+    <t>HVAC. Energy consumption of actuators in the fron-end were investigated. SARIMA model is identified: composing of ARMA and seasonal ARMA. Defrost cycles needed to be ignored. Segmented linear trends were assumed for modelling (to overcome nonlinearity). Single treshold is used, and for evaluation Gscor=sqrt(precision x recall). Without using sensors, the results were note convincing, but including them increased performance.</t>
+  </si>
+  <si>
+    <t>In this project every sensor got their own Q test threshold. 8 sensor measurement and the chiller energy balance equations were used. SCREE test is used to find the optimal number of principal components. It is empirically shown that the condenser temperatures have bigger range than the evaporator ones. Outlier are removed again.</t>
+  </si>
+  <si>
+    <t>Chiller. Lars's half empirical half analytic model is used for modelling. Model is discretized and the residual is normalized by variance. CUSUM is applied. Two isolation method are determined. One sensor per filter is better for isolating multiple fault scenarios, while filter applied for all but one sensor is more robust to plant deviations (Isermann, 2006). Multiple Model Adaptive Estimation (this is likelihood maximization based) is used. Extended version worked better than linear.</t>
+  </si>
+  <si>
+    <t>Chiller. UIO is used, conditions are stated then Lars's model is applied. Wide variety of conditions were tested, UIO did not work well during the nights. UIO was undercompeting against KF for sensor fault isolation, but overcompeting in parametric fault isolation. Detections were similarly effective.</t>
+  </si>
+  <si>
+    <t>Low charge detection with Eureqa</t>
+  </si>
+  <si>
+    <t>Non-ciritically charged refrigeration systems are fault diagnosed by the Eureqa sofware. The symbolic regression is an evolutionary computation method based that looks into space for a mathematical expression.  while minimizing different error metrics. Low and middle temperature level data are trained independently.</t>
+  </si>
+  <si>
+    <t>Logistic Regression, decision trees and random forest (ensemble model of decision tree with bagging and subspace sampling) are tested on industrial refrigeration system. The last one outperfromed the others in F1-score.</t>
+  </si>
+  <si>
+    <t>HVAC. The same sensors are used as in the virtual sensor articles (half analytic half experimental models). Support vector regression is used to fit nonlinearities more. CART algorithm creates the trees  Pruning is applied against overfitting, and expert knowledge rules are also used for pruning.  Confusion matrix, accuracy are used for evaluation. Tests on varying operating conditions but different training conditions give 69.18% accuracy.</t>
+  </si>
+  <si>
+    <t>https://findit.dtu.dk/en/catalog/245596364</t>
+  </si>
+  <si>
+    <t>HVAC. Data based technique: Q boundary rule is used to find new trends in the PC subspace. It was trained in normal operation by removing rows not fitting the normal assumption. This resulted in a less conservative threshold. False positives were not evaluated. Steady state detection is used.</t>
+  </si>
+  <si>
+    <t>It is shown, that the variables in refrigeration systems are rather non Gaussian, with Shapiro-Wilk test. Eight or 16 variables are used to compare to PCA-PC subspace methods. It outperforms it, pbecause PCA assumes Gaussian distribution, linear process variables, and is not adapting to several operating conditions.</t>
+  </si>
+  <si>
+    <t>PCA-R-SVDD based chiller fault detection</t>
+  </si>
+  <si>
+    <t>https://findit.dtu.dk/en/catalog/2290056945</t>
+  </si>
+  <si>
+    <t>The following methods are compared: PCA, SVDD, PCA-PC-SVDD and PCA-R-SVDD. For PCA, here not only the Q, but T (transformation or so called score matrix) boundaries are introduced. For PCA-X-SVDD, SVDD is applied on the subspaces, then the analytic equations of the two methods are merged. There are hyperparameters for SVDD, which need to be tuned with 10-fold cross validation. Kernel is Gaussian. The confidence level of fault detection is emprically assigned to 95%. The disadvantages of SVDD are described: cannot take uncertainty into consideration, higher FAR for training on data with limited operating conditions, high computational complexity. Steady state detection of Rossi with forgetting factor is used. For less severe fault levels, PCA-R-SVDD outperforms its competitors.</t>
+  </si>
+  <si>
+    <t>https://findit.dtu.dk/en/catalog/2435491725</t>
+  </si>
+  <si>
+    <t>PCA-R-BN fault detection for chillers</t>
+  </si>
+  <si>
+    <t>Since BN does not have good detection accuracies for low fault levels, PCA-R-BN architecture was tested. It is compared to PCA, PCA-PC, and BN. Two levels are used to define probability layers, fault and sympton levels, then the principle of the maximum posterior probability was used. Maximum likelihood is used to find the conditional probability parameters, and expert knowledge is used to find prior probability parameters.  The distance rejection model of Verron et al. was used to detect faults. Nine variables are selected for detection. The methods were tested on a physical plant.</t>
+  </si>
+  <si>
+    <t>Steady-state-signal identification</t>
+  </si>
+  <si>
+    <t>https://findit.dtu.dk/en/catalog/6529977</t>
+  </si>
+  <si>
+    <t>Online method for calculating variance; then, with well adjusted window size, physical HVAC signals were investigated, while the thresholds for standard deviation begin tuned. Different entering and leaving levels are used. It is shown taht in case of fault (refrigerant undercharge), the method is still operating correctly.</t>
   </si>
 </sst>
 </file>
@@ -573,31 +645,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:F39"/>
+  <dimension ref="C1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="63.21875" customWidth="1"/>
+    <col min="3" max="3" width="54.21875" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.44140625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -607,8 +683,11 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -618,8 +697,11 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -629,8 +711,11 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -643,323 +728,403 @@
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>17</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="F14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D14">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
         <v>40</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>49</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>60</v>
+      <c r="C36" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -976,30 +1141,31 @@
     <hyperlink ref="E12" r:id="rId10" xr:uid="{70F8D0E5-483B-44C6-92D3-08A750434D4D}"/>
     <hyperlink ref="E13" r:id="rId11" xr:uid="{A2FAD0B4-876F-46D7-B118-BD1D46B25B33}"/>
     <hyperlink ref="E14" r:id="rId12" xr:uid="{DF90D611-2B56-4B4F-9D81-F1F954B1C5F0}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{AB872264-65B3-4B0A-8207-D74C7A4C4C25}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{AB872264-65B3-4B0A-8207-D74C7A4C4C25}"/>
     <hyperlink ref="F6" r:id="rId14" xr:uid="{3BE3BD5E-7290-4A1B-836B-3546145B7C57}"/>
-    <hyperlink ref="F28" r:id="rId15" xr:uid="{30908C41-4A49-43F6-B884-12C798E4C613}"/>
-    <hyperlink ref="E18" r:id="rId16" xr:uid="{7ED5BCDA-3182-4A3A-B128-E033AE4792EA}"/>
-    <hyperlink ref="E19" r:id="rId17" xr:uid="{FA0AD573-382B-436C-80D8-CEA04AB28B5B}"/>
-    <hyperlink ref="E20" r:id="rId18" xr:uid="{DE92D924-EA49-439C-B874-D83CBFC40524}"/>
-    <hyperlink ref="E21" r:id="rId19" xr:uid="{9C236987-348E-4EDF-8257-92D1936D486B}"/>
-    <hyperlink ref="E22" r:id="rId20" xr:uid="{E326261C-7F45-4F4F-9975-FA87808F018B}"/>
-    <hyperlink ref="E30" r:id="rId21" xr:uid="{4058D00A-CFBC-42BB-BFB2-C88647459492}"/>
-    <hyperlink ref="E26" r:id="rId22" xr:uid="{0A63F6B1-AFFC-442F-9AD0-F57E89E1F9C9}"/>
-    <hyperlink ref="E27" r:id="rId23" xr:uid="{AC92FEAC-8CC3-4D05-A77F-433C313C03E6}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{2E72BA4C-CEE5-499C-8E9E-EB57A3B5419C}"/>
-    <hyperlink ref="E29" r:id="rId25" xr:uid="{7ED1B9C0-55E5-4117-84ED-2E337E187187}"/>
-    <hyperlink ref="E31" r:id="rId26" xr:uid="{2ECA15B0-13D3-4A68-BC3B-CF73E008E475}"/>
-    <hyperlink ref="E34" r:id="rId27" xr:uid="{AB678251-A8F1-499F-88C6-887279888DCB}"/>
-    <hyperlink ref="E35" r:id="rId28" xr:uid="{1DD78567-B40D-46C4-9905-99F154E72C2A}"/>
-    <hyperlink ref="E37" r:id="rId29" xr:uid="{DB0CF792-1115-4915-AA63-60FAF95D7CBB}"/>
-    <hyperlink ref="E38" r:id="rId30" xr:uid="{3BDD37B6-86C3-4F61-A0B9-132EA85F6C83}"/>
-    <hyperlink ref="E36" r:id="rId31" xr:uid="{3CB69D2B-1840-4DF0-81E6-9864F33E70E5}"/>
-    <hyperlink ref="F19" r:id="rId32" xr:uid="{85C843F2-348E-4DA7-83AB-EA87BBA50395}"/>
-    <hyperlink ref="E39" r:id="rId33" xr:uid="{B19988FD-E2DD-43E9-BCFB-8C4048679161}"/>
-    <hyperlink ref="E23" r:id="rId34" xr:uid="{DADF2E40-1E7B-4EE2-839D-CAF0201DCAA5}"/>
+    <hyperlink ref="F31" r:id="rId15" xr:uid="{30908C41-4A49-43F6-B884-12C798E4C613}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{7ED5BCDA-3182-4A3A-B128-E033AE4792EA}"/>
+    <hyperlink ref="E22" r:id="rId17" xr:uid="{FA0AD573-382B-436C-80D8-CEA04AB28B5B}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{DE92D924-EA49-439C-B874-D83CBFC40524}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{9C236987-348E-4EDF-8257-92D1936D486B}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{E326261C-7F45-4F4F-9975-FA87808F018B}"/>
+    <hyperlink ref="E33" r:id="rId21" xr:uid="{4058D00A-CFBC-42BB-BFB2-C88647459492}"/>
+    <hyperlink ref="E29" r:id="rId22" xr:uid="{0A63F6B1-AFFC-442F-9AD0-F57E89E1F9C9}"/>
+    <hyperlink ref="E30" r:id="rId23" xr:uid="{AC92FEAC-8CC3-4D05-A77F-433C313C03E6}"/>
+    <hyperlink ref="E31" r:id="rId24" xr:uid="{2E72BA4C-CEE5-499C-8E9E-EB57A3B5419C}"/>
+    <hyperlink ref="E32" r:id="rId25" xr:uid="{7ED1B9C0-55E5-4117-84ED-2E337E187187}"/>
+    <hyperlink ref="E34" r:id="rId26" xr:uid="{2ECA15B0-13D3-4A68-BC3B-CF73E008E475}"/>
+    <hyperlink ref="E37" r:id="rId27" xr:uid="{AB678251-A8F1-499F-88C6-887279888DCB}"/>
+    <hyperlink ref="E38" r:id="rId28" xr:uid="{1DD78567-B40D-46C4-9905-99F154E72C2A}"/>
+    <hyperlink ref="E40" r:id="rId29" xr:uid="{DB0CF792-1115-4915-AA63-60FAF95D7CBB}"/>
+    <hyperlink ref="E41" r:id="rId30" xr:uid="{3BDD37B6-86C3-4F61-A0B9-132EA85F6C83}"/>
+    <hyperlink ref="E39" r:id="rId31" xr:uid="{3CB69D2B-1840-4DF0-81E6-9864F33E70E5}"/>
+    <hyperlink ref="F22" r:id="rId32" xr:uid="{85C843F2-348E-4DA7-83AB-EA87BBA50395}"/>
+    <hyperlink ref="E42" r:id="rId33" xr:uid="{B19988FD-E2DD-43E9-BCFB-8C4048679161}"/>
+    <hyperlink ref="E25" r:id="rId34" xr:uid="{DADF2E40-1E7B-4EE2-839D-CAF0201DCAA5}"/>
+    <hyperlink ref="F14" r:id="rId35" xr:uid="{6B11D6A9-1E3A-4253-B9A0-CCCC780DC26D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>